<commit_message>
Login and Register w/ Profile Load
</commit_message>
<xml_diff>
--- a/Modelo-Relacional.xlsx
+++ b/Modelo-Relacional.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dashboard\BDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864D7879-139D-4249-B772-E5AFC601062A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07463CC1-B2F7-405D-8410-3882981AED2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
   <si>
     <t>Rol</t>
   </si>
@@ -129,9 +129,6 @@
     <t>idValoracion</t>
   </si>
   <si>
-    <t>puntiacion</t>
-  </si>
-  <si>
     <t>comentario</t>
   </si>
   <si>
@@ -181,6 +178,33 @@
   </si>
   <si>
     <t>idForma_Pago</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>idChat</t>
+  </si>
+  <si>
+    <t>Mensajes_Chat</t>
+  </si>
+  <si>
+    <t>idMensajes</t>
+  </si>
+  <si>
+    <t>mensaje</t>
+  </si>
+  <si>
+    <t>idComprador</t>
+  </si>
+  <si>
+    <t>idRemitente</t>
+  </si>
+  <si>
+    <t>puntuacion</t>
+  </si>
+  <si>
+    <t>precioCotizado</t>
   </si>
 </sst>
 </file>
@@ -204,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +239,12 @@
       <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -278,18 +308,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="33">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -307,7 +395,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color theme="8"/>
@@ -316,8 +410,6 @@
           <color theme="8"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -337,7 +429,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="8"/>
         </left>
@@ -346,9 +444,15 @@
           <color theme="8"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -367,7 +471,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color theme="8"/>
@@ -376,8 +486,6 @@
           <color theme="8"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -397,7 +505,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="8"/>
         </left>
@@ -406,9 +520,175 @@
           <color theme="8"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -424,28 +704,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{47BE8764-E0F1-4ABC-A168-1CE8EDC9F7E0}" name="Tabla3" displayName="Tabla3" ref="A1:B3" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{47BE8764-E0F1-4ABC-A168-1CE8EDC9F7E0}" name="Tabla3" displayName="Tabla3" ref="A1:B3" totalsRowShown="0" dataDxfId="32">
   <autoFilter ref="A1:B3" xr:uid="{47BE8764-E0F1-4ABC-A168-1CE8EDC9F7E0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4E6414FA-1E0E-4E19-8C3B-87D9AB2BDD76}" name="Rol"/>
-    <tableColumn id="2" xr3:uid="{F9F73611-6F03-4DC0-84AB-594556A2C241}" name="Columna1"/>
+    <tableColumn id="1" xr3:uid="{4E6414FA-1E0E-4E19-8C3B-87D9AB2BDD76}" name="Rol" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{F9F73611-6F03-4DC0-84AB-594556A2C241}" name="Columna1" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{63CAC8DB-6E53-48AA-A29A-A1D5535ED5EB}" name="Tabla131112" displayName="Tabla131112" ref="D19:E25" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{63CAC8DB-6E53-48AA-A29A-A1D5535ED5EB}" name="Tabla131112" displayName="Tabla131112" ref="D19:E25" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="D19:E25" xr:uid="{63CAC8DB-6E53-48AA-A29A-A1D5535ED5EB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F98DCA6B-46B7-4266-9C2D-785797393F73}" name="Compra_Producto" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{244018D5-3948-45DC-BAC1-81995969316B}" name="Columna1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F98DCA6B-46B7-4266-9C2D-785797393F73}" name="Compra_Producto" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{244018D5-3948-45DC-BAC1-81995969316B}" name="Columna1" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -466,28 +746,50 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3A314D0F-1DCD-4D16-B983-6F0565719764}" name="Tabla917" displayName="Tabla917" ref="J16:K20" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3A314D0F-1DCD-4D16-B983-6F0565719764}" name="Tabla917" displayName="Tabla917" ref="J16:K20" totalsRowShown="0" dataDxfId="15">
   <autoFilter ref="J16:K20" xr:uid="{3A314D0F-1DCD-4D16-B983-6F0565719764}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0C1396D1-6343-465F-884E-5C3C4732DB0D}" name="Lista_Producto"/>
-    <tableColumn id="2" xr3:uid="{B2D516C5-D796-40B8-8BA0-D3D9E40C1D40}" name="Columna1"/>
+    <tableColumn id="1" xr3:uid="{0C1396D1-6343-465F-884E-5C3C4732DB0D}" name="Lista_Producto" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{B2D516C5-D796-40B8-8BA0-D3D9E40C1D40}" name="Columna1" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFCB428B-17CB-4084-9B93-674286800161}" name="Tabla122" displayName="Tabla122" ref="M1:N3" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFCB428B-17CB-4084-9B93-674286800161}" name="Tabla122" displayName="Tabla122" ref="M1:N3" totalsRowShown="0" dataDxfId="12">
   <autoFilter ref="M1:N3" xr:uid="{BFCB428B-17CB-4084-9B93-674286800161}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{80CFCEF9-E245-4B38-8063-BA0E62D150A1}" name="Forma_Pago"/>
-    <tableColumn id="2" xr3:uid="{82C26191-E6F6-434F-887D-62D510768914}" name="Columna1"/>
+    <tableColumn id="1" xr3:uid="{80CFCEF9-E245-4B38-8063-BA0E62D150A1}" name="Forma_Pago" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{82C26191-E6F6-434F-887D-62D510768914}" name="Columna1" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71CC0ED0-0C06-418B-B7D3-7F48B27D8164}" name="Tabla1223" displayName="Tabla1223" ref="M5:N10" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="M5:N10" xr:uid="{71CC0ED0-0C06-418B-B7D3-7F48B27D8164}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{67B8A483-71F1-4360-9891-58052238771A}" name="Chat" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{75574A1F-D0A7-40E1-BCCD-44EDCCE8F859}" name="Columna1" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{053104B0-63B7-485F-89D9-94C53BD672BC}" name="Tabla1228" displayName="Tabla1228" ref="M12:N17" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="M12:N17" xr:uid="{053104B0-63B7-485F-89D9-94C53BD672BC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{187A9707-BEBB-4D86-9C5C-20A2C4BF3314}" name="Mensajes_Chat" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4B26AE04-E784-4166-B604-77E915A22B4A}" name="Columna1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -522,14 +824,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D169811D-E7F5-494B-84FD-2AFC5EFFE936}" name="Tabla6" displayName="Tabla6" ref="G11:H15" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D169811D-E7F5-494B-84FD-2AFC5EFFE936}" name="Tabla6" displayName="Tabla6" ref="G11:H15" totalsRowShown="0" dataDxfId="21">
   <autoFilter ref="G11:H15" xr:uid="{D169811D-E7F5-494B-84FD-2AFC5EFFE936}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0312356E-3B20-40C7-B7E4-426CF638E78A}" name="Categoria"/>
-    <tableColumn id="2" xr3:uid="{37B8BCBB-E013-40AB-9613-C97E3A0D7B9C}" name="Columna1"/>
+    <tableColumn id="1" xr3:uid="{0312356E-3B20-40C7-B7E4-426CF638E78A}" name="Categoria" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{37B8BCBB-E013-40AB-9613-C97E3A0D7B9C}" name="Columna1" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -550,56 +852,56 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1FE72CA5-2299-4634-A327-8A42B26343AF}" name="Tabla9" displayName="Tabla9" ref="G17:H21" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1FE72CA5-2299-4634-A327-8A42B26343AF}" name="Tabla9" displayName="Tabla9" ref="G17:H21" totalsRowShown="0" dataDxfId="18">
   <autoFilter ref="G17:H21" xr:uid="{1FE72CA5-2299-4634-A327-8A42B26343AF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A7F116A7-B275-4D76-A138-04584EA011A0}" name="Categoria_Producto"/>
-    <tableColumn id="2" xr3:uid="{3684DC6D-D8F1-4A84-AB73-8598A025C3E9}" name="Columna1"/>
+    <tableColumn id="1" xr3:uid="{A7F116A7-B275-4D76-A138-04584EA011A0}" name="Categoria_Producto" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{3684DC6D-D8F1-4A84-AB73-8598A025C3E9}" name="Columna1" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{844DBAE6-9A95-4AED-96D1-610CAC9A7F1A}" name="Tabla12" displayName="Tabla12" ref="G1:H4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{844DBAE6-9A95-4AED-96D1-610CAC9A7F1A}" name="Tabla12" displayName="Tabla12" ref="G1:H4" totalsRowShown="0" dataDxfId="27">
   <autoFilter ref="G1:H4" xr:uid="{844DBAE6-9A95-4AED-96D1-610CAC9A7F1A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{22B8A992-1E85-4E6A-9BA4-F055834D64D6}" name="Imagen"/>
-    <tableColumn id="2" xr3:uid="{1CB53E87-DC81-4CA7-BE91-7F789BCC5C1E}" name="Columna1"/>
+    <tableColumn id="1" xr3:uid="{22B8A992-1E85-4E6A-9BA4-F055834D64D6}" name="Imagen" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{1CB53E87-DC81-4CA7-BE91-7F789BCC5C1E}" name="Columna1" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{8E60FD75-B00C-441D-B192-2B019A2703E5}" name="Tabla13" displayName="Tabla13" ref="G6:H9" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{8E60FD75-B00C-441D-B192-2B019A2703E5}" name="Tabla13" displayName="Tabla13" ref="G6:H9" totalsRowShown="0" dataDxfId="24">
   <autoFilter ref="G6:H9" xr:uid="{8E60FD75-B00C-441D-B192-2B019A2703E5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4071A90C-9D59-4664-BF39-9DA5D0990AE8}" name="Video"/>
-    <tableColumn id="2" xr3:uid="{1BB6C59C-FFD7-474B-B67D-21D270AB80A4}" name="Columna1"/>
+    <tableColumn id="1" xr3:uid="{4071A90C-9D59-4664-BF39-9DA5D0990AE8}" name="Video" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{1BB6C59C-FFD7-474B-B67D-21D270AB80A4}" name="Columna1" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A52F54CF-905D-41CE-8F0C-31F41C3D535D}" name="Tabla1311" displayName="Tabla1311" ref="D12:E17" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A52F54CF-905D-41CE-8F0C-31F41C3D535D}" name="Tabla1311" displayName="Tabla1311" ref="D12:E17" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="D12:E17" xr:uid="{A52F54CF-905D-41CE-8F0C-31F41C3D535D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2E90768E-7C11-47F6-A367-9D0BA01B24F9}" name="Compra" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{F5A44B30-49EB-47BE-AC98-490C1E1CDE7D}" name="Columna1" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{2E90768E-7C11-47F6-A367-9D0BA01B24F9}" name="Compra" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{F5A44B30-49EB-47BE-AC98-490C1E1CDE7D}" name="Columna1" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -871,20 +1173,20 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="M13" sqref="M13:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.109375" customWidth="1"/>
     <col min="10" max="10" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.109375" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.109375" customWidth="1"/>
     <col min="16" max="16" width="12.5546875" customWidth="1"/>
     <col min="17" max="17" width="11.109375" customWidth="1"/>
@@ -916,74 +1218,81 @@
         <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="E3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="M3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
-      </c>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -992,210 +1301,290 @@
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J5" t="s">
+      <c r="E5" s="2"/>
+      <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="K5" s="2"/>
+      <c r="M5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="E6" s="2"/>
       <c r="G6" t="s">
         <v>17</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K6" t="s">
-        <v>13</v>
+      <c r="K6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
+      <c r="E7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K7" t="s">
-        <v>13</v>
-      </c>
+      <c r="K7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>49</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="G8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
+      <c r="E9" s="2"/>
+      <c r="G9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
       </c>
+      <c r="M9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
+      <c r="B10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="M10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B11" s="2"/>
       <c r="G11" t="s">
         <v>27</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B12" s="2"/>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K12" s="2"/>
+      <c r="M12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="B13" s="2"/>
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="D14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="E14" s="5"/>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="D15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="G15" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="H15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="J16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="M16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G17" t="s">
@@ -1204,105 +1593,113 @@
       <c r="H17" t="s">
         <v>20</v>
       </c>
-      <c r="J17" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="J17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="G18" t="s">
+      <c r="M17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J18" t="s">
-        <v>43</v>
-      </c>
-      <c r="K18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="J18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
         <v>20</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H19" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="H19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D20" s="2" t="s">
+      <c r="K19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="G21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H20" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="G21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="E24" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="13">
+  <tableParts count="15">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1316,6 +1713,8 @@
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>